<commit_message>
Delete ~$rticipant Survey Codebook.docx
</commit_message>
<xml_diff>
--- a/results/Table 1.xlsx
+++ b/results/Table 1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8040"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8040" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="40">
   <si>
     <t>Test Results</t>
   </si>
@@ -141,6 +141,24 @@
   </si>
   <si>
     <t>Variance Explained in Subjective Conclusions Results</t>
+  </si>
+  <si>
+    <t>Baseline Variance</t>
+  </si>
+  <si>
+    <t>Team-Levela (n = 87)</t>
+  </si>
+  <si>
+    <t>Model-Levela (n = 1,253)</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Belief in Hypothesis</t>
+  </si>
+  <si>
+    <t>Peer Model Ranking</t>
   </si>
 </sst>
 </file>
@@ -480,7 +498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -659,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -676,74 +694,74 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>14</v>
+      <c r="A6" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>16</v>
+      <c r="A8" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>17</v>
+      <c r="A9" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>20</v>
+      <c r="A12" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -753,12 +771,12 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>